<commit_message>
Updated to just re-upload the images instead of all of the product setup.
</commit_message>
<xml_diff>
--- a/uft_one_ai_aos_setup_otw_products/Default.xlsx
+++ b/uft_one_ai_aos_setup_otw_products/Default.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>Represents growth, harmony, and nature</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Red Kyber Crystal</t>
+  </si>
+  <si>
+    <t>Yellow Kyber Crystal</t>
+  </si>
+  <si>
+    <t>Yellow Kyber Crystal.jpg</t>
   </si>
   <si>
     <t>Darth Silious LLC</t>
@@ -696,7 +702,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -721,22 +727,22 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -753,16 +759,16 @@
         <v>84.989999999999995</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -785,13 +791,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -811,7 +817,7 @@
         <v>2499.9899999999998</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -820,13 +826,13 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3">
         <v>2500</v>
@@ -843,19 +849,19 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3">
         <v>2</v>
@@ -863,7 +869,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1">
         <v>179.99000000000001</v>
@@ -872,19 +878,19 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -892,7 +898,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1">
         <v>99.989999999999995</v>
@@ -901,23 +907,38 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -937,7 +958,7 @@
     <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>